<commit_message>
GZ-0465: PRODUCTS EXPORT ADDED
</commit_message>
<xml_diff>
--- a/src/test/resources/products.xlsx
+++ b/src/test/resources/products.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
   <si>
     <t xml:space="preserve">Product Name</t>
   </si>
@@ -55,36 +55,41 @@
     <t xml:space="preserve">99,99</t>
   </si>
   <si>
+    <t xml:space="preserve">/home/monika/Desktop/test-image.png
+https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRytuES2BfyGEuE_zFQi4l0kfbiy2LB__gH9cZIKsoh2D12tJQB
+https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRytuES2BfyGEuE_zFQi4l0kfbiy2LB__gH9cZIKsoh2D12tJQB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SK15987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electronics/phones/smart-phones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEST</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRytuES2BfyGEuE_zFQi4l0kfbiy2LB__gH9cZIKsoh2D12tJQB</t>
   </si>
   <si>
-    <t xml:space="preserve">SK15987</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">electronics/phones/smart-phones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100g</t>
-  </si>
-  <si>
-    <t xml:space="preserve">size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">color</t>
-  </si>
-  <si>
-    <t xml:space="preserve">black</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEST</t>
-  </si>
-  <si>
     <t xml:space="preserve">Smart watch</t>
   </si>
   <si>
@@ -92,6 +97,9 @@
   </si>
   <si>
     <t xml:space="preserve">15,99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/monika/Desktop/test-image.png</t>
   </si>
   <si>
     <t xml:space="preserve">SK123548</t>
@@ -209,8 +217,9 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -262,7 +271,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -280,19 +289,23 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -323,7 +336,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -331,7 +344,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="139.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="66.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="36.71"/>
@@ -386,7 +399,7 @@
       <c r="F2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -403,7 +416,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="6"/>
+      <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
         <v>17</v>
       </c>
@@ -411,14 +424,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="6"/>
+      <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
         <v>18</v>
       </c>
@@ -437,7 +450,7 @@
         <v>99.9</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>20</v>
@@ -445,7 +458,7 @@
       <c r="F5" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>14</v>
       </c>
       <c r="H5" s="0" t="s">
@@ -457,31 +470,31 @@
     </row>
     <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>11</v>
+        <v>24</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>25</v>
+      <c r="G6" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -491,12 +504,12 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="6"/>
+      <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -506,41 +519,41 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="6"/>
+      <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>11</v>
+        <v>35</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>35</v>
+      <c r="G9" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -549,13 +562,13 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="6"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -564,13 +577,13 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="6"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -579,13 +592,13 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="6"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -598,8 +611,8 @@
       <c r="C13" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>11</v>
+      <c r="D13" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>20</v>
@@ -607,7 +620,7 @@
       <c r="F13" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="6" t="s">
         <v>14</v>
       </c>
       <c r="H13" s="0" t="s">
@@ -643,10 +656,8 @@
     <mergeCell ref="G9:G12"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRytuES2BfyGEuE_zFQi4l0kfbiy2LB__gH9cZIKsoh2D12tJQB"/>
-    <hyperlink ref="D5" r:id="rId2" display="https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRytuES2BfyGEuE_zFQi4l0kfbiy2LB__gH9cZIKsoh2D12tJQB"/>
-    <hyperlink ref="D6" r:id="rId3" display="https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRytuES2BfyGEuE_zFQi4l0kfbiy2LB__gH9cZIKsoh2D12tJQB"/>
-    <hyperlink ref="D13" r:id="rId4" display="https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRytuES2BfyGEuE_zFQi4l0kfbiy2LB__gH9cZIKsoh2D12tJQB"/>
+    <hyperlink ref="D5" r:id="rId1" display="https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRytuES2BfyGEuE_zFQi4l0kfbiy2LB__gH9cZIKsoh2D12tJQB"/>
+    <hyperlink ref="D13" r:id="rId2" display="https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRytuES2BfyGEuE_zFQi4l0kfbiy2LB__gH9cZIKsoh2D12tJQB"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>